<commit_message>
Proyecto base finalizado. El exporter de estrategias está armado para que al seguir incluyendo nuevas estrategias, se siga exportando correctamente el excel base y las columnas necesarias puntuales de dicha estrategia se agregan al exporter. A su vez, se modularizo todo el proyecto. Quedo muy bien !!
</commit_message>
<xml_diff>
--- a/Resources/Summary.xlsx
+++ b/Resources/Summary.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,20 +552,20 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>GGAL.BA</t>
+          <t>SEMI.BA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
         <v>10000</v>
       </c>
       <c r="E2" t="n">
-        <v>19242.3473</v>
+        <v>65754.37359242247</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -573,280 +573,55 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45169</v>
+        <v>45170</v>
       </c>
       <c r="H2" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K2" t="n">
-        <v>0.375</v>
+        <v>0.333</v>
       </c>
       <c r="L2" t="n">
-        <v>0.625</v>
+        <v>0.667</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.189</v>
+        <v>-0.08699999999999999</v>
       </c>
       <c r="N2" t="n">
-        <v>1663.652</v>
+        <v>5709.358</v>
       </c>
       <c r="O2" t="n">
-        <v>0.161</v>
+        <v>0.271</v>
       </c>
       <c r="P2" t="n">
-        <v>-952.8920000000001</v>
+        <v>-1456.424</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.083</v>
+        <v>-0.06</v>
       </c>
       <c r="R2" t="n">
-        <v>-2524.492</v>
+        <v>-6238.426</v>
       </c>
       <c r="S2" t="n">
-        <v>6996.77</v>
+        <v>45693.333</v>
       </c>
       <c r="T2" t="n">
-        <v>0.699677</v>
+        <v>4.569333321689681</v>
       </c>
       <c r="U2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W2" t="n">
-        <v>36.07692307692308</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>MORI.BA</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E3" t="n">
-        <v>26932.96952342987</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2019-08-13</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>45169</v>
-      </c>
-      <c r="H3" t="n">
-        <v>55</v>
-      </c>
-      <c r="I3" t="n">
-        <v>13</v>
-      </c>
-      <c r="J3" t="n">
-        <v>42</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.236</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.764</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-0.14</v>
-      </c>
-      <c r="N3" t="n">
-        <v>4132.242</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.284</v>
-      </c>
-      <c r="P3" t="n">
-        <v>-1434.53</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>-0.063</v>
-      </c>
-      <c r="R3" t="n">
-        <v>-4742.102</v>
-      </c>
-      <c r="S3" t="n">
-        <v>22574.243</v>
-      </c>
-      <c r="T3" t="n">
-        <v>2.257424255013371</v>
-      </c>
-      <c r="U3" t="n">
-        <v>4</v>
-      </c>
-      <c r="V3" t="n">
-        <v>10</v>
-      </c>
-      <c r="W3" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>EDN.BA</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>12</v>
-      </c>
-      <c r="C4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>69278.1876</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2019-08-13</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>45169</v>
-      </c>
-      <c r="H4" t="n">
-        <v>36</v>
-      </c>
-      <c r="I4" t="n">
-        <v>12</v>
-      </c>
-      <c r="J4" t="n">
-        <v>24</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.333</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.667</v>
-      </c>
-      <c r="M4" t="n">
-        <v>-0.177</v>
-      </c>
-      <c r="N4" t="n">
-        <v>6374.792</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.346</v>
-      </c>
-      <c r="P4" t="n">
-        <v>-1139.04</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>-0.075</v>
-      </c>
-      <c r="R4" t="n">
-        <v>-3279.608</v>
-      </c>
-      <c r="S4" t="n">
-        <v>41817.298</v>
-      </c>
-      <c r="T4" t="n">
-        <v>4.181729760000001</v>
-      </c>
-      <c r="U4" t="n">
-        <v>2</v>
-      </c>
-      <c r="V4" t="n">
-        <v>13</v>
-      </c>
-      <c r="W4" t="n">
-        <v>40.02857142857143</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>YPFD.BA</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E5" t="n">
-        <v>47291.9844</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2019-08-13</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>45169</v>
-      </c>
-      <c r="H5" t="n">
-        <v>38</v>
-      </c>
-      <c r="I5" t="n">
-        <v>14</v>
-      </c>
-      <c r="J5" t="n">
-        <v>24</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.368</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.632</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-0.126</v>
-      </c>
-      <c r="N5" t="n">
-        <v>4269.058</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.243</v>
-      </c>
-      <c r="P5" t="n">
-        <v>-1480.89</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>-0.074</v>
-      </c>
-      <c r="R5" t="n">
-        <v>-4571.8</v>
-      </c>
-      <c r="S5" t="n">
-        <v>14970.234</v>
-      </c>
-      <c r="T5" t="n">
-        <v>1.49702343</v>
-      </c>
-      <c r="U5" t="n">
-        <v>3</v>
-      </c>
-      <c r="V5" t="n">
-        <v>7</v>
-      </c>
-      <c r="W5" t="n">
-        <v>38</v>
+        <v>34.26829268292683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregué la estrategia MACD. Agregué el gráfico de correlación, aunque por ahí habría que hacer más lindos los colores. Corregí para que represente correctamente los gráficos cuando se les pasa múltiples activos para analizar.
</commit_message>
<xml_diff>
--- a/Resources/Summary.xlsx
+++ b/Resources/Summary.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,20 +552,20 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>M.BA</t>
+          <t>BABA.BA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="n">
         <v>1000000</v>
       </c>
       <c r="E2" t="n">
-        <v>6387103.287225001</v>
+        <v>1359390.288</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -573,55 +573,280 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45183</v>
+        <v>45190</v>
       </c>
       <c r="H2" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I2" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J2" t="n">
         <v>15</v>
       </c>
       <c r="K2" t="n">
-        <v>0.464</v>
+        <v>0.348</v>
       </c>
       <c r="L2" t="n">
-        <v>0.536</v>
+        <v>0.652</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-0.158</v>
       </c>
       <c r="N2" t="n">
-        <v>428826.258</v>
+        <v>170013.286</v>
       </c>
       <c r="O2" t="n">
-        <v>0.188</v>
+        <v>0.208</v>
       </c>
       <c r="P2" t="n">
-        <v>-92574.789</v>
+        <v>-94548.67200000001</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.052</v>
+        <v>-0.101</v>
       </c>
       <c r="R2" t="n">
-        <v>-236304.743</v>
+        <v>-145094.332</v>
       </c>
       <c r="S2" t="n">
-        <v>2330591.91</v>
+        <v>351006.288</v>
       </c>
       <c r="T2" t="n">
-        <v>2.33059191015625</v>
+        <v>0.3510062880000002</v>
       </c>
       <c r="U2" t="n">
+        <v>3</v>
+      </c>
+      <c r="V2" t="n">
+        <v>7</v>
+      </c>
+      <c r="W2" t="n">
+        <v>53.36363636363637</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>BYMA.BA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3569549.789</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2019-08-13</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>45190</v>
+      </c>
+      <c r="H3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I3" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" t="n">
+        <v>14</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.417</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.583</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-0.075</v>
+      </c>
+      <c r="N3" t="n">
+        <v>369946.83</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-138062.594</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-302669.471</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1312411.312</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1.312411312</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3</v>
+      </c>
+      <c r="V3" t="n">
         <v>4</v>
       </c>
-      <c r="V2" t="n">
-        <v>6</v>
-      </c>
-      <c r="W2" t="n">
-        <v>53.2962962962963</v>
+      <c r="W3" t="n">
+        <v>61.73913043478261</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>PAMP.BA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3457455.821599243</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2019-08-13</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>45190</v>
+      </c>
+      <c r="H4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I4" t="n">
+        <v>14</v>
+      </c>
+      <c r="J4" t="n">
+        <v>18</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-0.165</v>
+      </c>
+      <c r="N4" t="n">
+        <v>265916.153</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-119193.557</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-241159.874</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1296548.942</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1.296548941523559</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3</v>
+      </c>
+      <c r="V4" t="n">
+        <v>4</v>
+      </c>
+      <c r="W4" t="n">
+        <v>43.03225806451613</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>YPFD.BA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5388942.6954</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2019-08-13</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>45190</v>
+      </c>
+      <c r="H5" t="n">
+        <v>27</v>
+      </c>
+      <c r="I5" t="n">
+        <v>14</v>
+      </c>
+      <c r="J5" t="n">
+        <v>13</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.519</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.481</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-0.232</v>
+      </c>
+      <c r="N5" t="n">
+        <v>435622.156</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.233</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-205632.772</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0.104</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-888172.085</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1476139.244</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1.4761392437</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3</v>
+      </c>
+      <c r="V5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W5" t="n">
+        <v>53.69230769230769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>